<commit_message>
kpi_table can be successfully exported.
</commit_message>
<xml_diff>
--- a/python/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/python/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_matlab/01_kpi_extractor/AEB_KPI_Project/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D519AB2D-D250-4448-9857-72B01F73110A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD01FB13-24E6-C348-8433-780333AEB5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4960" yWindow="7660" windowWidth="34200" windowHeight="13460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3500" windowWidth="34200" windowHeight="17180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -1101,7 +1101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1395,7 +1395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECBDC44-4FC0-EE44-827D-4641F2FAC044}">
   <dimension ref="B2:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -2008,9 +2008,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE39B99-0AFB-8547-83BF-D855CC6E3BB3}">
   <dimension ref="B1:G35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2280,7 +2280,7 @@
         <v>119</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>

</xml_diff>

<commit_message>
graphs can generated but PedalPosProIncrease_Th isn't visible
</commit_message>
<xml_diff>
--- a/python/config/SignalMap_KPI_PlotSpec.xlsx
+++ b/python/config/SignalMap_KPI_PlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_matlab/01_kpi_extractor/AEB_KPI_Project/python/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD01FB13-24E6-C348-8433-780333AEB5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61F54A4-0458-3B47-8650-9BA9E3C22CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3500" windowWidth="34200" windowHeight="17180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3500" windowWidth="34200" windowHeight="17180" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="217">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -131,15 +131,9 @@
     <t>vehSpd</t>
   </si>
   <si>
-    <t>m1DeadTime</t>
-  </si>
-  <si>
     <t>intvDur</t>
   </si>
   <si>
-    <t>pedalMax</t>
-  </si>
-  <si>
     <t>absSteerMaxDeg</t>
   </si>
   <si>
@@ -666,6 +660,36 @@
   </si>
   <si>
     <t xml:space="preserve">resample frequency </t>
+  </si>
+  <si>
+    <t>PedalPosPro</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Example Color</t>
+  </si>
+  <si>
+    <t>🔵 Deep Blue</t>
+  </si>
+  <si>
+    <t>🟠 Vivid Orange</t>
+  </si>
+  <si>
+    <t>🟢 Bright Green</t>
+  </si>
+  <si>
+    <t>🔴 Crimson</t>
+  </si>
+  <si>
+    <t>🟣 Purple</t>
+  </si>
+  <si>
+    <t>🟤 Brown</t>
+  </si>
+  <si>
+    <t>🌸 Pink</t>
   </si>
 </sst>
 </file>
@@ -758,7 +782,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -767,9 +791,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -785,6 +806,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1113,276 +1140,276 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="7" t="s">
+      <c r="B11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="7" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="B14" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="B15" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="10"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="10"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="10"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="10"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="10"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="10"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="10"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="10"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="9"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="10"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="9"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="10"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="10"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="9"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="10"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="10"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="9"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="10"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="10"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1406,154 +1433,154 @@
     <col min="6" max="6" width="44.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>185</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C3">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C5">
         <v>300</v>
       </c>
       <c r="D5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C6">
         <v>-6</v>
       </c>
       <c r="D6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C7">
         <v>-15</v>
       </c>
       <c r="D7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F7" t="s">
         <v>198</v>
-      </c>
-      <c r="F7" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C8">
         <v>-4.9000000000000004</v>
       </c>
       <c r="D8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C9">
         <v>0.2</v>
       </c>
       <c r="D9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C10">
         <v>0.01</v>
       </c>
       <c r="D10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1564,10 +1591,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24310F59-1486-4F41-B3B7-AB25CE8F592D}">
-  <dimension ref="B2:K14"/>
+  <dimension ref="B2:K15"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1583,9 +1610,9 @@
     <col min="11" max="11" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>10</v>
@@ -1600,7 +1627,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>14</v>
@@ -1612,12 +1639,12 @@
         <v>23</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>29</v>
@@ -1629,7 +1656,7 @@
         <v>85</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>16</v>
@@ -1638,7 +1665,7 @@
         <v>17</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>24</v>
@@ -1649,10 +1676,10 @@
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>101</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>175</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -1661,7 +1688,7 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G4" s="2" t="b">
         <v>1</v>
@@ -1670,7 +1697,7 @@
         <v>17</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>24</v>
@@ -1681,10 +1708,10 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -1693,16 +1720,16 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>24</v>
@@ -1713,10 +1740,10 @@
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>207</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>178</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -1725,7 +1752,7 @@
         <v>100</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G6" s="2" t="b">
         <v>1</v>
@@ -1734,7 +1761,7 @@
         <v>18</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>24</v>
@@ -1745,28 +1772,26 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>207</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>179</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
       </c>
       <c r="E7" s="3">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>43</v>
+      <c r="H7" s="2"/>
+      <c r="I7" s="12" t="s">
+        <v>148</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>24</v>
@@ -1777,28 +1802,28 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
       </c>
       <c r="E8" s="3">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G8" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>24</v>
@@ -1809,28 +1834,28 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
       </c>
       <c r="E9" s="3">
-        <v>40</v>
+        <v>600</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G9" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>24</v>
@@ -1841,28 +1866,28 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
       </c>
       <c r="E10" s="3">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="G10" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>24</v>
@@ -1873,51 +1898,51 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>84</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
       </c>
       <c r="E11" s="3">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G11" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="D12" s="3">
         <v>0</v>
       </c>
       <c r="E12" s="3">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G12" s="2" t="b">
         <v>1</v>
@@ -1926,7 +1951,7 @@
         <v>17</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>24</v>
@@ -1937,10 +1962,10 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="2" t="s">
         <v>80</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="D13" s="3">
         <v>0</v>
@@ -1949,7 +1974,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G13" s="2" t="b">
         <v>1</v>
@@ -1958,7 +1983,7 @@
         <v>17</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>24</v>
@@ -1969,10 +1994,10 @@
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="D14" s="3">
         <v>0</v>
@@ -1981,21 +2006,53 @@
         <v>5</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="K14" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>5</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2008,9 +2065,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE39B99-0AFB-8547-83BF-D855CC6E3BB3}">
   <dimension ref="B1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2024,627 +2081,627 @@
     <col min="7" max="7" width="45.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" s="12" t="s">
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" s="13" t="s">
+      <c r="E4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="D4" s="13" t="s">
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="D5" s="13" t="s">
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="D6" s="13" t="s">
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="D7" s="13" t="s">
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="13" t="s">
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" s="13" t="s">
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D13" s="13" t="s">
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13" t="s">
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C30" s="13" t="s">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E32" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="D30" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="G30" s="13" t="s">
+      <c r="F32" s="12"/>
+      <c r="G32" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B31" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13" t="s">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B33" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C33" s="13" t="s">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13" t="s">
+      <c r="D35" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2657,54 +2714,54 @@
   <dimension ref="B1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2714,100 +2771,152 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1943DE-263B-CE4F-869C-DE791D333F1F}">
-  <dimension ref="B2:D9"/>
+  <dimension ref="B2:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0.44700000000000001</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="F2" s="13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14">
+        <v>0.121</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="14">
+        <v>2</v>
+      </c>
+      <c r="C4" s="14">
+        <v>1</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0.498</v>
+      </c>
+      <c r="E4" s="14">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="14">
+        <v>3</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.627</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="14">
+        <v>4</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0.153</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.157</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="14">
+        <v>5</v>
+      </c>
+      <c r="C7" s="14">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D7" s="14">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="E7" s="14">
         <v>0.74099999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="5">
-        <v>0.85</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="D4" s="5">
-        <v>9.8000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="5">
-        <v>0.92900000000000005</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0.69399999999999995</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="5">
-        <v>0.49399999999999999</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0.184</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.55600000000000005</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="5">
+      <c r="F7" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="14">
+        <v>6</v>
+      </c>
+      <c r="C8" s="14">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="14">
+        <v>7</v>
+      </c>
+      <c r="C9" s="14">
+        <v>0.89</v>
+      </c>
+      <c r="D9" s="14">
         <v>0.46600000000000003</v>
       </c>
-      <c r="C7" s="5">
-        <v>0.67400000000000004</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0.188</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="5">
-        <v>0.30099999999999999</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0.745</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.93300000000000005</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="5">
-        <v>0.63500000000000001</v>
-      </c>
-      <c r="C9" s="5">
-        <v>7.8E-2</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0.184</v>
+      <c r="E9" s="14">
+        <v>0.76</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>